<commit_message>
Write CSV File about Monitoring OS Disk Usage result
</commit_message>
<xml_diff>
--- a/report/DB관리대장_종합_2021.10.xlsx
+++ b/report/DB관리대장_종합_2021.10.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="102">
   <si>
     <t>DB Check List</t>
   </si>
@@ -278,6 +278,66 @@
   <si>
     <t>88%</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65%</t>
+  </si>
+  <si>
+    <t>31%</t>
+  </si>
+  <si>
+    <t>66%</t>
+  </si>
+  <si>
+    <t>29%</t>
+  </si>
+  <si>
+    <t>51%</t>
+  </si>
+  <si>
+    <t>88%</t>
+  </si>
+  <si>
+    <t>35%</t>
+  </si>
+  <si>
+    <t>27%</t>
+  </si>
+  <si>
+    <t>92.0%</t>
+  </si>
+  <si>
+    <t>89.0%</t>
+  </si>
+  <si>
+    <t>94.0%</t>
+  </si>
+  <si>
+    <t>98.0%</t>
+  </si>
+  <si>
+    <t>88.0%</t>
+  </si>
+  <si>
+    <t>20.0%</t>
+  </si>
+  <si>
+    <t>92%%</t>
+  </si>
+  <si>
+    <t>89%%</t>
+  </si>
+  <si>
+    <t>94%%</t>
+  </si>
+  <si>
+    <t>98%%</t>
+  </si>
+  <si>
+    <t>88%%</t>
+  </si>
+  <si>
+    <t>20%%</t>
   </si>
 </sst>
 </file>
@@ -1082,8 +1142,12 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="M8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -1583,8 +1647,12 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
+      <c r="M19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
@@ -2084,8 +2152,12 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+      <c r="M30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
@@ -2538,8 +2610,12 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+      <c r="M40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
@@ -2585,8 +2661,12 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
+      <c r="M41" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
@@ -2632,8 +2712,12 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
+      <c r="M42" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
@@ -2679,8 +2763,12 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
+      <c r="M43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
@@ -2726,8 +2814,12 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
+      <c r="M44" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
@@ -2773,8 +2865,12 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
+      <c r="M45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>

</xml_diff>

<commit_message>
Write CSV File about Monitoring Table Space Usage Result
</commit_message>
<xml_diff>
--- a/report/DB관리대장_종합_2021.10.xlsx
+++ b/report/DB관리대장_종합_2021.10.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="109">
   <si>
     <t>DB Check List</t>
   </si>
@@ -338,6 +338,27 @@
   </si>
   <si>
     <t>20%%</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
+    <t>53%</t>
+  </si>
+  <si>
+    <t>38%</t>
+  </si>
+  <si>
+    <t>93%</t>
+  </si>
+  <si>
+    <t>28%</t>
+  </si>
+  <si>
+    <t>42%</t>
+  </si>
+  <si>
+    <t>43%</t>
   </si>
 </sst>
 </file>
@@ -1148,7 +1169,9 @@
       <c r="N8" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="O8" s="2"/>
+      <c r="O8" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -1653,7 +1676,9 @@
       <c r="N19" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="O19" s="2"/>
+      <c r="O19" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
@@ -2158,7 +2183,9 @@
       <c r="N30" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="O30" s="2"/>
+      <c r="O30" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
@@ -2616,7 +2643,9 @@
       <c r="N40" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="O40" s="2"/>
+      <c r="O40" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
@@ -2667,7 +2696,9 @@
       <c r="N41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="O41" s="2"/>
+      <c r="O41" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
@@ -2718,7 +2749,9 @@
       <c r="N42" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="O42" s="2"/>
+      <c r="O42" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
@@ -2769,7 +2802,9 @@
       <c r="N43" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="O43" s="2"/>
+      <c r="O43" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
@@ -2820,7 +2855,9 @@
       <c r="N44" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="O44" s="2"/>
+      <c r="O44" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
@@ -2871,7 +2908,9 @@
       <c r="N45" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="O45" s="2"/>
+      <c r="O45" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>

</xml_diff>

<commit_message>
Write CSV File about Monitoring Archive Usage Result
</commit_message>
<xml_diff>
--- a/report/DB관리대장_종합_2021.10.xlsx
+++ b/report/DB관리대장_종합_2021.10.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="109">
   <si>
     <t>DB Check List</t>
   </si>
@@ -1172,7 +1172,9 @@
       <c r="O8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="P8" s="2"/>
+      <c r="P8" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
@@ -1679,7 +1681,9 @@
       <c r="O19" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="P19" s="2"/>
+      <c r="P19" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -2186,7 +2190,9 @@
       <c r="O30" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="P30" s="2"/>
+      <c r="P30" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>

</xml_diff>

<commit_message>
Write CSV File about Monitoring ASM Disk Usage Result
</commit_message>
<xml_diff>
--- a/report/DB관리대장_종합_2021.10.xlsx
+++ b/report/DB관리대장_종합_2021.10.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="115">
   <si>
     <t>DB Check List</t>
   </si>
@@ -359,6 +359,24 @@
   </si>
   <si>
     <t>43%</t>
+  </si>
+  <si>
+    <t>39%</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>26%</t>
+  </si>
+  <si>
+    <t>47%</t>
+  </si>
+  <si>
+    <t>41%</t>
+  </si>
+  <si>
+    <t>44%</t>
   </si>
 </sst>
 </file>
@@ -1173,10 +1191,14 @@
         <v>108</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
+        <v>107</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
@@ -1682,10 +1704,14 @@
         <v>103</v>
       </c>
       <c r="P19" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q19" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
+      <c r="R19" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
@@ -2191,10 +2217,14 @@
         <v>85</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
+        <v>106</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
@@ -2652,9 +2682,15 @@
       <c r="O40" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
+      <c r="P40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R40" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
@@ -2705,9 +2741,15 @@
       <c r="O41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="P41" s="2"/>
-      <c r="Q41" s="2"/>
-      <c r="R41" s="2"/>
+      <c r="P41" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="R41" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
@@ -2758,9 +2800,15 @@
       <c r="O42" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-      <c r="R42" s="2"/>
+      <c r="P42" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="R42" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
@@ -2811,9 +2859,15 @@
       <c r="O43" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="P43" s="2"/>
-      <c r="Q43" s="2"/>
-      <c r="R43" s="2"/>
+      <c r="P43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="R43" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
@@ -2864,9 +2918,15 @@
       <c r="O44" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
-      <c r="R44" s="2"/>
+      <c r="P44" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="R44" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
@@ -2917,9 +2977,15 @@
       <c r="O45" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
-      <c r="R45" s="2"/>
+      <c r="P45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>

</xml_diff>